<commit_message>
Party Master added in Transation IN forms
</commit_message>
<xml_diff>
--- a/Dinesh Demo Project/ColdStorage/Task Cold Storage.xlsx
+++ b/Dinesh Demo Project/ColdStorage/Task Cold Storage.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
   <si>
     <t>Priority</t>
   </si>
@@ -76,6 +76,18 @@
   </si>
   <si>
     <t>Show Amount in report and price in</t>
+  </si>
+  <si>
+    <t>Party Master in Transation IN form</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>In progress</t>
+  </si>
+  <si>
+    <t>Party Master in Transation Out form</t>
   </si>
 </sst>
 </file>
@@ -407,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -542,6 +554,34 @@
       </c>
       <c r="E8" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Transatin IN master add party details
</commit_message>
<xml_diff>
--- a/Dinesh Demo Project/ColdStorage/Task Cold Storage.xlsx
+++ b/Dinesh Demo Project/ColdStorage/Task Cold Storage.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
   <si>
     <t>Priority</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>Party Master in Transation Out form</t>
+  </si>
+  <si>
+    <t>pending in reports</t>
   </si>
 </sst>
 </file>
@@ -419,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -435,7 +438,7 @@
     <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -455,7 +458,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
@@ -472,7 +475,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>2</v>
       </c>
@@ -489,7 +492,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>3</v>
       </c>
@@ -503,7 +506,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>4</v>
       </c>
@@ -517,7 +520,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>5</v>
       </c>
@@ -531,7 +534,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>6</v>
       </c>
@@ -545,7 +548,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>7</v>
       </c>
@@ -556,7 +559,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>8</v>
       </c>
@@ -567,10 +570,13 @@
         <v>21</v>
       </c>
       <c r="F9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>18</v>
+      </c>
+      <c r="G9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
Change for New Master, DEtails and LOokup for Item master
</commit_message>
<xml_diff>
--- a/Dinesh Demo Project/ColdStorage/Task Cold Storage.xlsx
+++ b/Dinesh Demo Project/ColdStorage/Task Cold Storage.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
   <si>
     <t>Priority</t>
   </si>
@@ -91,6 +91,24 @@
   </si>
   <si>
     <t>pending in reports</t>
+  </si>
+  <si>
+    <t>ItemMasterDetails, Lookup multple value, Item Maste Add Edit single forms</t>
+  </si>
+  <si>
+    <t>Party master</t>
+  </si>
+  <si>
+    <t>Multple selection in Transation forms</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> In Progress</t>
   </si>
 </sst>
 </file>
@@ -422,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -463,97 +481,86 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" t="s">
-        <v>16</v>
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
         <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
       </c>
       <c r="E6" t="s">
         <v>16</v>
       </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E7" t="s">
         <v>16</v>
       </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
         <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
       </c>
       <c r="E8" t="s">
         <v>16</v>
@@ -561,33 +568,94 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>20</v>
+      <c r="C9" t="s">
+        <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
         <v>23</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E14" t="s">
         <v>21</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F14" t="s">
         <v>22</v>
+      </c>
+      <c r="G14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Canges done for Party master lookup
</commit_message>
<xml_diff>
--- a/Dinesh Demo Project/ColdStorage/Task Cold Storage.xlsx
+++ b/Dinesh Demo Project/ColdStorage/Task Cold Storage.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -114,8 +114,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,6 +152,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -198,7 +206,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -230,9 +238,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -264,6 +273,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -439,24 +449,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -476,7 +486,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -490,7 +500,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -504,7 +514,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -518,7 +528,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -535,7 +545,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2</v>
       </c>
@@ -552,7 +562,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>3</v>
       </c>
@@ -566,7 +576,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>4</v>
       </c>
@@ -580,7 +590,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>5</v>
       </c>
@@ -594,7 +604,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>6</v>
       </c>
@@ -608,7 +618,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>7</v>
       </c>
@@ -619,7 +629,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>8</v>
       </c>
@@ -636,7 +646,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>9</v>
       </c>
@@ -653,7 +663,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>10</v>
       </c>
@@ -664,24 +674,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>